<commit_message>
Adding details and new figures for paper
</commit_message>
<xml_diff>
--- a/hardware/final_bom.xlsx
+++ b/hardware/final_bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub Repos\canine_precise_dispenser\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E209ED-0F99-4313-A0FF-ACB4D6E3120F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD5FABD-8AB1-4EEF-9411-C50BDF780192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
   <si>
     <t>Bill of Materials - Precise Dispenser</t>
   </si>
@@ -130,6 +130,60 @@
   </si>
   <si>
     <t>Power Switch</t>
+  </si>
+  <si>
+    <t>Used to print the dispenser</t>
+  </si>
+  <si>
+    <t>Use</t>
+  </si>
+  <si>
+    <t>Controls the dispenser</t>
+  </si>
+  <si>
+    <t>Breaks out HDMI connection on Pi to connector panel</t>
+  </si>
+  <si>
+    <t>Breaks out 5V USB power on Pi to connector panel</t>
+  </si>
+  <si>
+    <t>Breaks out 12V power on Pi HAT to connector panel</t>
+  </si>
+  <si>
+    <t>Converts the HDMI panel connector to Micro HDMI on Pi</t>
+  </si>
+  <si>
+    <t>12V power supply for stepper motor</t>
+  </si>
+  <si>
+    <t>Motor to drive the treat jogger</t>
+  </si>
+  <si>
+    <t>5V power supply for Raspberry Pi</t>
+  </si>
+  <si>
+    <t>Acrylic plate to cover the treats from the environment</t>
+  </si>
+  <si>
+    <t>External sensors to detect a treat falling from jogger</t>
+  </si>
+  <si>
+    <t>Used to hold down wires within the dispenser</t>
+  </si>
+  <si>
+    <t>Used to hold data and OS on Raspberry Pi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connects the panel USB C to Raspberry Pi </t>
+  </si>
+  <si>
+    <t>Double pull double throw switch for both 5V and 12V power</t>
+  </si>
+  <si>
+    <t>Placed on Pi HAT into the female headers</t>
+  </si>
+  <si>
+    <t>Soldered to Pi HAT</t>
   </si>
 </sst>
 </file>
@@ -232,7 +286,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -250,6 +304,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -634,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -646,7 +701,7 @@
     <col min="4" max="4" width="44.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -654,7 +709,7 @@
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -667,8 +722,11 @@
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -685,8 +743,11 @@
       <c r="E3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -703,8 +764,11 @@
       <c r="E4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -721,8 +785,11 @@
       <c r="E5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -739,8 +806,11 @@
       <c r="E6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -757,8 +827,11 @@
       <c r="E7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
@@ -775,8 +848,11 @@
       <c r="E8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
@@ -793,8 +869,11 @@
       <c r="E9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
@@ -811,8 +890,11 @@
       <c r="E10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
@@ -829,8 +911,11 @@
       <c r="E11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>17</v>
       </c>
@@ -847,8 +932,11 @@
       <c r="E12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
@@ -865,8 +953,11 @@
       <c r="E13" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>20</v>
       </c>
@@ -883,8 +974,11 @@
       <c r="E14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>21</v>
       </c>
@@ -901,8 +995,11 @@
       <c r="E15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>22</v>
       </c>
@@ -919,8 +1016,11 @@
       <c r="E16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>31</v>
       </c>
@@ -937,8 +1037,11 @@
       <c r="E17" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>23</v>
       </c>
@@ -955,8 +1058,11 @@
       <c r="E18" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>24</v>
       </c>
@@ -974,8 +1080,11 @@
       <c r="E19" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>25</v>
       </c>
@@ -992,8 +1101,11 @@
       <c r="E20" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>26</v>
       </c>
@@ -1010,8 +1122,11 @@
       <c r="E21" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>27</v>
       </c>
@@ -1028,8 +1143,11 @@
       <c r="E22" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>28</v>
       </c>
@@ -1046,8 +1164,11 @@
       <c r="E23" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>29</v>
       </c>
@@ -1064,8 +1185,11 @@
       <c r="E24" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>30</v>
       </c>
@@ -1082,6 +1206,9 @@
       </c>
       <c r="E25" t="s">
         <v>10</v>
+      </c>
+      <c r="F25" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>